<commit_message>
added tee to BOM
</commit_message>
<xml_diff>
--- a/variations/Camden/V0.2/BOM-SPARC-Camden-v0.2.xlsx
+++ b/variations/Camden/V0.2/BOM-SPARC-Camden-v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\Smart-Pack-for-Advanced-Research-and-Control\variations\Camden\V0.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4948E9E3-1F9A-4168-B6E9-8091640239FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF99E11-5D5D-4100-9245-755C08B289FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="15840" xr2:uid="{FDAE7DA4-9528-4FC7-A320-70DA50473DCE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Total Cost</t>
   </si>
@@ -357,6 +357,15 @@
   </si>
   <si>
     <t>https://www.aliexpress.us/item/3256805148780496.html?gatewayAdapt=glo2usa4itemAdapt</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/AIGNEP-USA-Tee-Nickel-Plated-Brass-1CPF4?opr=ODOH&amp;analytics=FM:Order%20History</t>
+  </si>
+  <si>
+    <t>Tee: Nickel-Plated Brass, 1/4 in x 1/4 in x 1/4 in Fitting Pipe Size, 2 in Overall Lg</t>
+  </si>
+  <si>
+    <t>1/4 in Tee</t>
   </si>
 </sst>
 </file>
@@ -762,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D3A36C-E8CE-4E50-A172-E48E2F9A45A8}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +864,7 @@
         <v>9.99</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E32" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E33" si="0">C3*D3</f>
         <v>9.99</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1513,12 +1522,25 @@
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="4"/>
+      <c r="A33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2</v>
+      </c>
+      <c r="D33" s="6">
+        <v>6.06</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="0"/>
+        <v>12.12</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -1538,7 +1560,7 @@
       </c>
       <c r="E35" s="6">
         <f>SUM(E2:E34)</f>
-        <v>12404.389999999996</v>
+        <v>12416.509999999997</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="5"/>
@@ -1615,8 +1637,10 @@
     <hyperlink ref="F30" r:id="rId28" display="https://www.digikey.com/en/products/detail/belden-inc/35618-002500/7041945?gclsrc=aw.ds&amp;gad_source=1&amp;gad_campaignid=22518541616&amp;gbraid=0AAAAADrbLljEBpjA6o11517XtnCbKLnsR&amp;gclid=Cj0KCQjwuKnGBhD5ARIsAD19Rsa4nb1dzOV49q-F9Xe7dRzLg9fr09jgomA5Q7py5DmHjVBe4NA0heoaAspGEALw_wcB" xr:uid="{A2DDC80C-6F39-4C44-B776-452B7FA8CAC3}"/>
     <hyperlink ref="F31" r:id="rId29" xr:uid="{71E7E2F7-3EA3-469E-BDBD-A5E1E2E4F347}"/>
     <hyperlink ref="F32" r:id="rId30" xr:uid="{F2165E25-79D9-4521-9261-0FF86CB8CEB1}"/>
+    <hyperlink ref="F11" r:id="rId31" xr:uid="{2459F536-6BF7-4F95-8ED6-65EBE68E0306}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{A1AFF2B0-3BCF-4EB1-A5D8-3277D679C9A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>